<commit_message>
fix error httpclient doesnot send request
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="148">
   <si>
     <t>User</t>
   </si>
@@ -402,9 +402,6 @@
     <t>Device - Specification</t>
   </si>
   <si>
-    <t>specification_id</t>
-  </si>
-  <si>
     <t>device - id</t>
   </si>
   <si>
@@ -457,13 +454,22 @@
   </si>
   <si>
     <t xml:space="preserve"> Specification</t>
+  </si>
+  <si>
+    <t>devicetype</t>
+  </si>
+  <si>
+    <t>spection_name</t>
+  </si>
+  <si>
+    <t>value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -519,8 +525,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color theme="2" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -560,6 +573,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -637,7 +656,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -673,9 +692,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -728,6 +744,18 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1034,7 +1062,7 @@
   <dimension ref="A1:S96"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,51 +1095,51 @@
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="P2" s="15" t="s">
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="P2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
     </row>
     <row r="3" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="18"/>
-      <c r="F3" s="17" t="s">
+      <c r="A3" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="17"/>
+      <c r="F3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
       <c r="K3" s="1"/>
       <c r="P3" s="3" t="s">
         <v>2</v>
@@ -1127,61 +1155,61 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="F4" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="G4" s="23" t="s">
+      <c r="F4" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="G4" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="I4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="18"/>
+      <c r="J4" s="17"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="18"/>
-      <c r="B5" s="22" t="s">
+      <c r="A5" s="17"/>
+      <c r="B5" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22" t="s">
+      <c r="E5" s="21"/>
+      <c r="F5" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="G5" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="18"/>
+      <c r="G5" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="17"/>
       <c r="K5" s="1"/>
       <c r="P5" s="3" t="s">
         <v>35</v>
@@ -1191,32 +1219,32 @@
       </c>
     </row>
     <row r="6" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="18"/>
-      <c r="B6" s="22" t="s">
+      <c r="A6" s="17"/>
+      <c r="B6" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="F6" s="37" t="s">
+      <c r="F6" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="H6" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="22" t="s">
+      <c r="I6" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="18"/>
+      <c r="J6" s="17"/>
       <c r="K6" s="1"/>
       <c r="P6" s="2" t="s">
         <v>85</v>
@@ -1226,30 +1254,30 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22" t="s">
+      <c r="B7" s="21"/>
+      <c r="C7" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="F7" s="37" t="s">
+      <c r="F7" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="18"/>
-      <c r="H7" s="22" t="s">
+      <c r="G7" s="17"/>
+      <c r="H7" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="I7" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="18"/>
+      <c r="J7" s="17"/>
       <c r="K7" s="1"/>
       <c r="P7" s="2" t="s">
         <v>86</v>
@@ -1259,159 +1287,159 @@
       </c>
     </row>
     <row r="8" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A8" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="22" t="s">
+      <c r="A8" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="18"/>
-      <c r="H8" s="22" t="s">
+      <c r="G8" s="17"/>
+      <c r="H8" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="I8" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="J8" s="18"/>
+      <c r="J8" s="17"/>
       <c r="P8" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="G9" s="18"/>
-      <c r="H9" s="24" t="s">
+      <c r="G9" s="17"/>
+      <c r="H9" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="I9" s="22" t="s">
+      <c r="I9" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="18"/>
+      <c r="J9" s="17"/>
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="24" t="s">
+      <c r="B10" s="26"/>
+      <c r="C10" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24" t="s">
+      <c r="D10" s="23"/>
+      <c r="E10" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="24" t="s">
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="22" t="s">
+      <c r="I10" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="27"/>
+      <c r="J10" s="26"/>
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="24" t="s">
+      <c r="A11" s="26"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="24" t="s">
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="I11" s="22" t="s">
+      <c r="I11" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="J11" s="27"/>
+      <c r="J11" s="26"/>
       <c r="K11" s="1"/>
     </row>
     <row r="12" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="22" t="s">
+      <c r="A12" s="26"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="E12" s="18"/>
-      <c r="F12" s="17" t="s">
+      <c r="E12" s="17"/>
+      <c r="F12" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="H12" s="22" t="s">
+      <c r="G12" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="H12" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="I12" s="18"/>
-      <c r="J12" s="27"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="26"/>
       <c r="K12" s="1"/>
       <c r="P12" s="11" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="29" t="s">
+      <c r="B13" s="26"/>
+      <c r="C13" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="E13" s="18"/>
-      <c r="F13" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="18"/>
-      <c r="H13" s="24" t="s">
+      <c r="E13" s="17"/>
+      <c r="F13" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="17"/>
+      <c r="H13" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="I13" s="18"/>
-      <c r="J13" s="25" t="s">
-        <v>130</v>
+      <c r="I13" s="17"/>
+      <c r="J13" s="24" t="s">
+        <v>129</v>
       </c>
       <c r="K13" s="1"/>
       <c r="P13" s="8" t="s">
@@ -1419,28 +1447,28 @@
       </c>
     </row>
     <row r="14" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A14" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="24" t="s">
+      <c r="A14" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="26"/>
+      <c r="C14" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="D14" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="E14" s="17" t="s">
+      <c r="D14" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="E14" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="F14" s="26" t="s">
+      <c r="F14" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="18"/>
-      <c r="H14" s="24" t="s">
+      <c r="G14" s="17"/>
+      <c r="H14" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="I14" s="18"/>
-      <c r="J14" s="22" t="s">
+      <c r="I14" s="17"/>
+      <c r="J14" s="21" t="s">
         <v>16</v>
       </c>
       <c r="P14" s="8" t="s">
@@ -1448,560 +1476,564 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A15" s="26" t="s">
-        <v>139</v>
-      </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="24" t="s">
+      <c r="A15" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="B15" s="26"/>
+      <c r="C15" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="E15" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="22" t="s">
+      <c r="E15" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="18"/>
-      <c r="H15" s="24" t="s">
+      <c r="G15" s="17"/>
+      <c r="H15" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="18"/>
-      <c r="J15" s="22" t="s">
+      <c r="I15" s="17"/>
+      <c r="J15" s="21" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="31" t="s">
+      <c r="B16" s="26"/>
+      <c r="C16" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="D16" s="22" t="s">
-        <v>138</v>
-      </c>
-      <c r="E16" s="24" t="s">
+      <c r="D16" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="E16" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="22" t="s">
+      <c r="F16" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="G16" s="18"/>
-      <c r="H16" s="22" t="s">
+      <c r="G16" s="17"/>
+      <c r="H16" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="I16" s="17"/>
+      <c r="J16" s="26"/>
+    </row>
+    <row r="17" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A17" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="26"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="I16" s="18"/>
-      <c r="J16" s="27"/>
-    </row>
-    <row r="17" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A17" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="29" t="s">
+      <c r="I17" s="17"/>
+      <c r="J17" s="26"/>
+      <c r="P17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A18" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="26"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="26"/>
+      <c r="P18" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A19" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="F19" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="G19" s="17"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="P19" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A20" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="26"/>
+      <c r="C20" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="17"/>
+      <c r="E20" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="G20" s="17"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+    </row>
+    <row r="21" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A21" s="21"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="17"/>
+      <c r="E21" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="40" t="s">
+        <v>124</v>
+      </c>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+    </row>
+    <row r="22" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A22" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="26"/>
+      <c r="C22" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="F22" s="17"/>
+      <c r="G22" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="H22" s="17"/>
+      <c r="I22" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="J22" s="17"/>
+    </row>
+    <row r="23" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A23" s="23"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" s="17"/>
+      <c r="I23" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="J23" s="17"/>
+    </row>
+    <row r="24" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A24" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="26"/>
+      <c r="C24" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="17"/>
+      <c r="I24" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="J24" s="26"/>
+    </row>
+    <row r="25" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A25" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="26"/>
+      <c r="C25" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="J25" s="26"/>
+    </row>
+    <row r="26" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A26" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="26"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="J26" s="17"/>
+    </row>
+    <row r="27" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A27" s="17"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="J27" s="17"/>
+    </row>
+    <row r="28" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A28" s="17"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="F28" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="J28" s="17"/>
+    </row>
+    <row r="29" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A29" s="17"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="F29" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" s="17"/>
+      <c r="H29" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="I17" s="18"/>
-      <c r="J17" s="27"/>
-      <c r="P17" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A18" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="27"/>
-      <c r="P18" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A19" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="F19" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="G19" s="18"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="P19" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A20" s="22" t="s">
+      <c r="I29" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="J29" s="17"/>
+    </row>
+    <row r="30" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D30" s="17"/>
+      <c r="E30" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="F30" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G30" s="17"/>
+      <c r="H30" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="J30" s="17"/>
+    </row>
+    <row r="31" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A31" s="17"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="G31" s="17"/>
+      <c r="H31" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
+    </row>
+    <row r="32" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A32" s="17"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+    </row>
+    <row r="33" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A33" s="17"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="J33" s="17"/>
+    </row>
+    <row r="34" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A34" s="17"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="J34" s="17"/>
+    </row>
+    <row r="35" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A35" s="17"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="J35" s="17"/>
+    </row>
+    <row r="36" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A36" s="17"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="J36" s="17"/>
+    </row>
+    <row r="37" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A37" s="17"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="22" t="s">
-        <v>125</v>
-      </c>
-      <c r="G20" s="18"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-    </row>
-    <row r="21" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A21" s="22"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-    </row>
-    <row r="22" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A22" s="22" t="s">
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="17"/>
+      <c r="J37" s="17"/>
+    </row>
+    <row r="38" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A38" s="17"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="H22" s="18"/>
-      <c r="I22" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="J22" s="18"/>
-    </row>
-    <row r="23" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A23" s="24"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="24" t="s">
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="17"/>
+      <c r="J38" s="17"/>
+    </row>
+    <row r="39" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A39" s="17"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="G39" s="17"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="17"/>
+      <c r="J39" s="17"/>
+    </row>
+    <row r="40" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A40" s="17"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G40" s="17"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="17"/>
+      <c r="J40" s="17"/>
+    </row>
+    <row r="41" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A41" s="17"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="G41" s="17"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="17"/>
+      <c r="J41" s="17"/>
+    </row>
+    <row r="42" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A42" s="17"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="G42" s="17"/>
+      <c r="H42" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="I42" s="17"/>
+      <c r="J42" s="17"/>
+    </row>
+    <row r="43" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A43" s="17"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="I43" s="17"/>
+      <c r="J43" s="17"/>
+    </row>
+    <row r="44" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A44" s="17"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="I44" s="17"/>
+      <c r="J44" s="17"/>
+    </row>
+    <row r="45" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A45" s="17"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="17"/>
+      <c r="H45" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="H23" s="18"/>
-      <c r="I23" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="J23" s="18"/>
-    </row>
-    <row r="24" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A24" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="27"/>
-      <c r="C24" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="H24" s="18"/>
-      <c r="I24" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="J24" s="27"/>
-    </row>
-    <row r="25" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A25" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="B25" s="27"/>
-      <c r="C25" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="J25" s="27"/>
-    </row>
-    <row r="26" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A26" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="J26" s="18"/>
-    </row>
-    <row r="27" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A27" s="18"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="J27" s="18"/>
-    </row>
-    <row r="28" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A28" s="18"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="F28" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="J28" s="18"/>
-    </row>
-    <row r="29" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A29" s="18"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="F29" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="G29" s="18"/>
-      <c r="H29" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="I29" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="J29" s="18"/>
-    </row>
-    <row r="30" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A30" s="18"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="G30" s="18"/>
-      <c r="H30" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="I30" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="J30" s="18"/>
-    </row>
-    <row r="31" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A31" s="18"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="G31" s="18"/>
-      <c r="H31" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I31" s="18"/>
-      <c r="J31" s="18"/>
-    </row>
-    <row r="32" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A32" s="18"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-    </row>
-    <row r="33" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A33" s="18"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="G33" s="18"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="J33" s="18"/>
-    </row>
-    <row r="34" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="G34" s="18"/>
-      <c r="H34" s="18"/>
-      <c r="I34" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="J34" s="18"/>
-    </row>
-    <row r="35" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A35" s="18"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="G35" s="18"/>
-      <c r="H35" s="18"/>
-      <c r="I35" s="34" t="s">
-        <v>119</v>
-      </c>
-      <c r="J35" s="18"/>
-    </row>
-    <row r="36" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A36" s="18"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="G36" s="18"/>
-      <c r="H36" s="18"/>
-      <c r="I36" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="J36" s="18"/>
-    </row>
-    <row r="37" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A37" s="18"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="G37" s="18"/>
-      <c r="H37" s="18"/>
-      <c r="I37" s="18"/>
-      <c r="J37" s="18"/>
-    </row>
-    <row r="38" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A38" s="18"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="22" t="s">
+      <c r="I45" s="17"/>
+      <c r="J45" s="17"/>
+    </row>
+    <row r="46" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A46" s="17"/>
+      <c r="B46" s="17"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
-      <c r="J38" s="18"/>
-    </row>
-    <row r="39" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A39" s="18"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
-      <c r="J39" s="18"/>
-    </row>
-    <row r="40" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A40" s="18"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
-      <c r="J40" s="18"/>
-    </row>
-    <row r="41" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A41" s="18"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="18"/>
-    </row>
-    <row r="42" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A42" s="18"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="G42" s="18"/>
-      <c r="H42" s="35" t="s">
-        <v>117</v>
-      </c>
-      <c r="I42" s="18"/>
-      <c r="J42" s="18"/>
-    </row>
-    <row r="43" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A43" s="18"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="21" t="s">
-        <v>118</v>
-      </c>
-      <c r="I43" s="18"/>
-      <c r="J43" s="18"/>
-    </row>
-    <row r="44" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A44" s="18"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="G44" s="18"/>
-      <c r="H44" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="I44" s="18"/>
-      <c r="J44" s="18"/>
-    </row>
-    <row r="45" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A45" s="18"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="18"/>
-      <c r="H45" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="I45" s="18"/>
-      <c r="J45" s="18"/>
-    </row>
-    <row r="46" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A46" s="18"/>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="17"/>
+      <c r="J46" s="17"/>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">

</xml_diff>